<commit_message>
Update scripts directory and CCS documentation
</commit_message>
<xml_diff>
--- a/nanni_maize_2022/documentation/map_ccs_reads.xlsx
+++ b/nanni_maize_2022/documentation/map_ccs_reads.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHARE\McIntyre_Lab\maize_ozone_FINAL\2018\PacBio\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F9A9FA-A491-429A-86B0-A1D7BBB350E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A462CF3-7CF7-4F74-B57D-C7996095B2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="20736" windowHeight="10752" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -267,31 +267,7 @@
     <t>Assess CCS and cluster mapped identity and coverage</t>
   </si>
   <si>
-    <t xml:space="preserve">Count mapped CCS and mapped clusters based on identity and coverage of mapping
-NOTE: CCS sam file already filtered for supp alignments and unmapped
-NOTE: cluster sam file needs filtered for supp alignments and unmapped (-F 2052)
-samtools view -e  = expression used to filter alignments for certain values
-    [NM] is from the NM tag which is a count of mismatches to the reference
-    rlen is the length of the reference alignment
-    qlen is the length of the read
-</t>
-  </si>
-  <si>
     <t>samtools/1.12</t>
-  </si>
-  <si>
-    <t>$PROJ/scripts/pacbio/submit_asses_ccs_cluster_map_id_coverage.sbatch</t>
-  </si>
-  <si>
-    <t>$PROJ/check_isoseq3_lost_genes/minimap2/${SAMPLE_NAME}_minimap2_b73.sam
-$PROJ/compare_b73_2_mo17/mapping_minimap2_b73/${GENO}/${TRT}/${SAMPLE_NAME}.polished.all.hq.mapped.sam
-SAMPLE_NAME=${ID}_${GENO}_${TRT}=[19_mo17_amb,46_b73_oz,89_nc338_amb,113_c123_amb,21_mo17_oz,70_hp301_oz,96_nc338_oz,120_c123_oz,67_hp301_amb,42_b73_amb,21-2_mo17_oz]
-GENO = b73, c123, hp301, mo17, nc338</t>
-  </si>
-  <si>
-    <t>$PROJ/compare_b73_2_mo17/ccs_cluster_map_id_cov/
-ccs_map_id_cov_counts.csv
-cluster_map_id_cov_counts.csv</t>
   </si>
   <si>
     <t>genotype                           =     [b73, c123, hp301, mo17, nc338]
@@ -682,6 +658,33 @@
   <si>
     <t>make.flag_detect_cvrg_cnts_ccs
 /nfshome/ammorse/mclab/SHARE/McIntyre_Lab/maize_ozone_FINAL/make_combination_flag_file/flag_detect_cvrg_cnts_ccs.csv</t>
+  </si>
+  <si>
+    <t>$PROJ/scripts/pacbio/submit_asses_ccs_cluster_map_id_coverage_02avn.sbatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For each set of alignments to B73/Mo17 YAN/Mo17 CAU:
+Count mapped CCS and mapped clusters based on identity and coverage of mapping
+NOTE: CCS sam file already filtered for supp alignments and unmapped
+NOTE: cluster sam file needs filtered for supp alignments and unmapped (-F 2052)
+samtools view -e  = expression used to filter alignments for certain values
+    [NM] is from the NM tag which is a count of mismatches to the reference
+    rlen is the length of the reference alignment
+    qlen is the length of the read
+</t>
+  </si>
+  <si>
+    <t>$PROJ/check_isoseq3_lost_genes/minimap2/${SAMPLE_NAME}_minimap2_${REF}.sam
+$PROJ/compare_b73_2_mo17/mapping_minimap2_${REF}/${GENO}/${TRT}/${SAMPLE_NAME}.polished.all.hq.mapped.sam
+SAMPLE_NAME=${ID}_${GENO}_${TRT}=[19_mo17_amb,46_b73_oz,89_nc338_amb,113_c123_amb,21_mo17_oz,70_hp301_oz,96_nc338_oz,120_c123_oz,67_hp301_amb,42_b73_amb,21-2_mo17_oz]
+GENO = b73, c123, hp301, mo17, nc338
+REF=b73, mo17_yan, mo17_cau</t>
+  </si>
+  <si>
+    <t>$PROJ/compare_b73_2_mo17/ccs_cluster_map_id_cov/
+ccs_map_id_cov_counts_2_${REF}.csv
+cluster_map_id_cov_counts_2_${REF}.csv
+REF=b73, mo17_yan, mo17_cau</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1223,7 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,7 +1307,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1349,7 +1352,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1373,7 +1376,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -1491,22 +1494,22 @@
         <v>15</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>33</v>
@@ -1515,64 +1518,64 @@
     <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:8" s="7" customFormat="1" ht="360" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:8" s="7" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:8" s="7" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1603,7 +1606,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" s="7" customFormat="1" ht="288" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="7" customFormat="1" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>15</v>
       </c>
@@ -1611,22 +1614,22 @@
         <v>55</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="E30" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1635,22 +1638,22 @@
         <v>15</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="G32" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>33</v>
@@ -1662,22 +1665,22 @@
         <v>15</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>33</v>
@@ -1689,22 +1692,22 @@
         <v>15</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>33</v>
@@ -1716,22 +1719,22 @@
         <v>15</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>50</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1740,70 +1743,70 @@
         <v>15</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="41" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="43" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B44" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1812,22 +1815,22 @@
         <v>15</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="G46" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>47</v>
@@ -1836,46 +1839,46 @@
     <row r="47" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:8" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:10" s="7" customFormat="1" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="C50" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D50" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="E50" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="G48" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:10" s="7" customFormat="1" ht="403.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B50" s="7" t="s">
+      <c r="F50" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="G50" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="H50" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>